<commit_message>
add template and batch insert
</commit_message>
<xml_diff>
--- a/helper/template-taut.xlsx
+++ b/helper/template-taut.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\taut\backend\helper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E5EE9B9-9F7A-4902-B45A-FB780AA868C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000112EE-2FBE-4E06-A69E-859D72368A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{9BB95283-744C-439C-817A-FB1774A9934B}"/>
   </bookViews>
@@ -39,10 +39,10 @@
     <t>jabatan/pekerjaan</t>
   </si>
   <si>
-    <t>no. telp</t>
-  </si>
-  <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>no.telp</t>
   </si>
 </sst>
 </file>
@@ -78,8 +78,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,18 +398,18 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="17.44140625" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -416,8 +417,8 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
change template and insert batch
</commit_message>
<xml_diff>
--- a/helper/template-taut.xlsx
+++ b/helper/template-taut.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\taut\backend\helper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000112EE-2FBE-4E06-A69E-859D72368A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4BB833-8DB0-4DA4-AA94-A8B6CE72ED3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{9BB95283-744C-439C-817A-FB1774A9934B}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>username</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>nama</t>
   </si>
@@ -43,6 +40,18 @@
   </si>
   <si>
     <t>no.telp</t>
+  </si>
+  <si>
+    <t>nama organisasi / perusahaan :</t>
+  </si>
+  <si>
+    <t>Alias nama organisasi / perusahaan :</t>
+  </si>
+  <si>
+    <t>(isi alias disini)</t>
+  </si>
+  <si>
+    <t>(isi nama disini)</t>
   </si>
 </sst>
 </file>
@@ -58,12 +67,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -78,9 +105,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,39 +428,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F023DBDF-6036-432F-8AC5-4076B908A7FF}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="4.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
     <col min="3" max="3" width="17.44140625" customWidth="1"/>
     <col min="4" max="4" width="13.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" customWidth="1"/>
+    <col min="8" max="8" width="17.21875" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E4" s="4" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>